<commit_message>
promo short billboards update for this week
</commit_message>
<xml_diff>
--- a/cadence.xlsx
+++ b/cadence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur.lurye/Documents/automateHeroBanners/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur.lurye/Documents/cadence-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA18524A-C5E2-AF49-AAE8-B2C51704A928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C31E86A-4D69-6F4C-84D1-2294F54B12EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="1820" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
+    <workbookView xWindow="2600" yWindow="1660" windowWidth="29240" windowHeight="16940" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Promo Short Billboard" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -63,6 +63,9 @@
     <t>brandDescription</t>
   </si>
   <si>
+    <t>50% OFF</t>
+  </si>
+  <si>
     <t>20% OFF</t>
   </si>
   <si>
@@ -72,15 +75,6 @@
     <t>Shop Now</t>
   </si>
   <si>
-    <t>BOIRON_BOGO50_1203_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>BOGO 50% Off Boiron Supplements</t>
-  </si>
-  <si>
-    <t>Fight flu-like symptoms with homeopathic Oscillococcinum, Chestal for kids, and more.</t>
-  </si>
-  <si>
     <t>brandName</t>
   </si>
   <si>
@@ -237,116 +231,152 @@
     <t>BodyTech</t>
   </si>
   <si>
-    <t>S_2002_FROZEN20 20p off 75</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id : '2002_FROZEN20 20p off 75 Hero Banner', position : 'Hero Banner', name : '2002_FROZEN20 20p off 75', creative: '20% Off'})"</t>
-  </si>
-  <si>
     <t>/c/best-sellers/N-cp99qp</t>
   </si>
   <si>
-    <t>FROZEN20Coupon_Web_L3</t>
-  </si>
-  <si>
-    <t>your order of $75 or more</t>
-  </si>
-  <si>
     <t>/p/amino-energy-collagen-grape-remix-9-5-oz-powder/op-1242</t>
   </si>
   <si>
-    <t>NaturesPlus_BOGO50_012720_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>Optimum_BOGO50_012720_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>GardenofLife_20off_012720_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Natures Plus BOGO50 Promotional Short Billboard 1', position : 'Promotional Short Billboard 1', name : '2002_Natures Plus BOGO50', creative: 'BOGO50'})"</t>
-  </si>
-  <si>
     <t>/b/natures-plus/N-97w</t>
   </si>
   <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Optimum Amino Energy plus collagen BOGO50 Promotional Short Billboard 2', position : 'Promotional Short Billboard 2', name : '2002_Optimum Amino Energy plus collagen BOGO50', creative: 'BOGO50'})"</t>
-  </si>
-  <si>
     <t>/b/optimum-nutrition-performance-supplements/N-991Zcp99ja</t>
   </si>
   <si>
-    <t>ng-click="asset.promoClick({id :  '2002_GOL Dr Formulated Raw Probiotics 20p off Promotional Short Billboard 3', position : 'Promotional Short Billboard 3', name : '2002_GOL Dr Formulated Raw Probiotics 20p off', creative: '20% Off'})"</t>
-  </si>
-  <si>
-    <t>/b/garden-of-life-digestion/N-93uZcp99jm</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Nugenix 20p off Promotional Short Billboard 4', position : 'Promotional Short Billboard 4', name : '2002_Nugenix 20p off', creative: '20% Off'})"</t>
-  </si>
-  <si>
-    <t>/b/nugenix/N-cp982s</t>
-  </si>
-  <si>
-    <t>BOGO 50% Off NaturesPlus Supplements</t>
-  </si>
-  <si>
-    <t>Everybody needs a great multi. Get yours with Acai,  Resveratrol, &amp; 120+ whole foods!</t>
-  </si>
-  <si>
-    <t>BOGO 50% Off AMIN.O. Energy By Optimum Nutrition</t>
-  </si>
-  <si>
-    <t>Support focus &amp; recovery—now available with UC-II&lt;sup&gt;&amp;reg;&lt;/sup&gt; Collagen, clinically shown to improve joint comfort &amp; mobility!</t>
-  </si>
-  <si>
-    <t>20% Off Dr. Formulated &amp; Raw Probiotics</t>
-  </si>
-  <si>
-    <t>Save on probiotics from Garden of Life for digestive balance and immune health. Because your wellbeing is worth it.</t>
-  </si>
-  <si>
     <t>postHeaderText2</t>
   </si>
   <si>
     <t>postHeaderText3</t>
   </si>
   <si>
-    <t>PLUS FREE SHIPPING</t>
-  </si>
-  <si>
-    <t>Online Only | Use code: &lt;span&gt;FROZEN20&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>S_2002_GAMEPLAN 10d off 40 BOPUS</t>
-  </si>
-  <si>
     <t>ng-click="asset.promoClick({id :  '2002_GAMEPLAN 10d off 40 BOPUS Hero Banner', position : 'Hero Banner', name : '2002_GAMEPLAN 10d off 40 BOPUS', creative: '$10 Off'})"</t>
   </si>
   <si>
-    <t>GAMEPLANCoupon_Web_L3</t>
-  </si>
-  <si>
-    <t>SCORE $10 OFF</t>
-  </si>
-  <si>
-    <t>your order of $40 or more with 2-Hour Pickup *</t>
-  </si>
-  <si>
-    <t>Use code: &lt;span&gt;GAMEPLAN&lt;/span&gt;</t>
-  </si>
-  <si>
     <t>icon</t>
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>S_2002_VSB BOGO50 V1</t>
+  </si>
+  <si>
+    <t>S_2002_BT and BTE 20p off</t>
+  </si>
+  <si>
+    <t>S_2002_Natures Plus BOGO50</t>
+  </si>
+  <si>
+    <t>S_2002_Optimum Amino Energy plus collagen BOGO50</t>
+  </si>
+  <si>
+    <t>BOGO50VSB_012720_Web_L3</t>
+  </si>
+  <si>
+    <t>BodytechBTE_20off_012720_Web_L3</t>
+  </si>
+  <si>
+    <t>NaturesPlus_BOGO50_012720_Web_L3</t>
+  </si>
+  <si>
+    <t>Optimum_BOGO50_012720_Web_L3</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_VSB BOGO50 V1 Hero Banner', position : 'Hero Banner', name : '2002_VSB BOGO50 V1', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>BUY ONE, GET ONE</t>
+  </si>
+  <si>
+    <t>The Vitamin Shoppe&lt;sup&gt;&amp;reg;&lt;/sup&gt; brand supplements</t>
+  </si>
+  <si>
+    <t>BodyTech&lt;sup&gt;&amp;reg;&lt;/sup&gt; &amp;amp; BodyTech&lt;sup&gt;&amp;reg;&lt;/sup&gt; brand sports nutrition</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id : '2002_Natures Plus BOGO50 Hero Banner', position : 'Hero Banner', name : '2002_Natures Plus BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>NaturesPlus supplements</t>
+  </si>
+  <si>
+    <t>all Optimum Nutrition AMIN.O Energy products&lt;br&gt; featuring AMIN.O Energy Plus UC-11&lt;sup&gt;&amp;reg;&lt;/sup&gt; Collagen</t>
+  </si>
+  <si>
+    <t>Nourish yourself, inside and out. with naturally-sourced products from top beauty brands including Reserveage!</t>
+  </si>
+  <si>
+    <t>SHOP SALE &gt;</t>
+  </si>
+  <si>
+    <t>SHOP NOW &gt;</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_Optimum Amino Energy plus collagen BOGO50 Hero Banner', position : 'Hero Banner', name : '2002_Optimum Amino Energy plus collagen BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>/b/women-s-best/N-cp9a6g</t>
+  </si>
+  <si>
+    <t>WEB WK8 021720 Digestive Event 105625_Web_SecondaryBillboard</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_4 Day Digestive event 20p off Promotional Short Billboard 1', position : 'Promotional Short Billboard 1', name : '2002_4 Day Digestive event 20p off', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>/c/digestive-health-sale/N-cp99y8</t>
+  </si>
+  <si>
+    <t>Limited Time Only: Up To 20% Off Digestive Support</t>
+  </si>
+  <si>
+    <t>Nourish your gut with the right mix of probiotic strains featuring active bacterial cultures.</t>
+  </si>
+  <si>
+    <t>WomensBestLaunch_BOGO50_020320_SecondaryBillboard_01</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_Womens Best Launch and BOGO50 Promotional Short Billboard 2', position : 'Promotional Short Billboard 2', name : '2002_Womens Best Launch and BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>BOGO 50% Off NEW Women's Best&lt;sup&gt;&amp;trade;&lt;/sup&gt; Premium Supplements</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_Solaray Leaf therapeutics cbd 20p off Promotional Short Billboard 3', position : 'Promotional Short Billboard 3', name : '2002_Solaray Leaf therapeutics cbd 20p off', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>/c/cbd-hemp-extract/solaray/N-cp9a1pZ9b0</t>
+  </si>
+  <si>
+    <t>SOLARAY_20OFF_012720_Web_SecondaryBillboard</t>
+  </si>
+  <si>
+    <t>20% Off Leaf Therapeutics Hemp Extract By Solaray</t>
+  </si>
+  <si>
+    <t>Explore hemp extract for balance—plus targeted blends for pain &amp; sleep—with a full spectrum array of beneficial phytocannabinoids.</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2002_Jocko Lauch Promotional Short Billboard 4', position : 'Promotional Short Billboard 4', name : '2002_Jocko Lauch', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>/b/jocko-fuel/N-cp9a4i</t>
+  </si>
+  <si>
+    <t>Jocko_newbrandlaunch_012720_Web_SecondaryBillboard</t>
+  </si>
+  <si>
+    <t>Introducing Jocko Fuel</t>
+  </si>
+  <si>
+    <t>Built to work. Made for life. These new supplements are backed by science &amp; developed with retired Navy Seal Jocko Willink.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,11 +411,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -445,16 +470,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,11 +795,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FEE12E-A1B2-7945-8CDA-9BE45F21A83A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -798,83 +829,83 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>77</v>
+      <c r="A2" t="s">
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>79</v>
+      <c r="A3" t="s">
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -886,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCEFC6D-EE13-EF4B-A2EA-D63CE352C75D}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -926,10 +957,10 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -937,67 +968,107 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G4" s="2"/>
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G5" s="2"/>
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="3"/>
@@ -1042,10 +1113,10 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -1053,162 +1124,162 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>2151256</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
       </c>
       <c r="D3">
         <v>2198141</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>2193134</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>72</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>2194546</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>2148294</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>2189876</v>
       </c>
       <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>2189215</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>2172005</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1227,61 +1298,61 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding deal drawer main template
</commit_message>
<xml_diff>
--- a/cadence.xlsx
+++ b/cadence.xlsx
@@ -2,21 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur.lurye/Documents/cadence-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9FA020-5055-FB4F-ABE3-E06A2CE23753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3025C9B4-678C-8C42-A746-DB5008E37E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="1560" windowWidth="29240" windowHeight="16940" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
+    <workbookView xWindow="14700" yWindow="0" windowWidth="18900" windowHeight="21000" activeTab="2" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Html Ads" sheetId="9" r:id="rId1"/>
     <sheet name="heroBanners" sheetId="10" r:id="rId2"/>
+    <sheet name="Cross Promos" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
   <si>
     <t>name</t>
   </si>
@@ -263,13 +265,190 @@
   </si>
   <si>
     <t>2-AQ WK 10 STOPBY10_728X90_copy</t>
+  </si>
+  <si>
+    <t>bgColor</t>
+  </si>
+  <si>
+    <t>promo</t>
+  </si>
+  <si>
+    <t>cta</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>2003_Bang Candy Apple CPCM</t>
+  </si>
+  <si>
+    <t>2003_Apparel Get in Gear CPCM</t>
+  </si>
+  <si>
+    <t>2003_10 Ways Women Can Support Fertility CPCM</t>
+  </si>
+  <si>
+    <t>2003_Black Seed Oil CPCM</t>
+  </si>
+  <si>
+    <t>2003_Browse Videos CPCM</t>
+  </si>
+  <si>
+    <t>2003_Welcome to CBD Centeral CPCM</t>
+  </si>
+  <si>
+    <t>2003_Curious About CBD CPCM</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Bang Candy Apple Cross Promo Module', position : 'Cross Promo Module', name : '2003_Bang Candy Apple', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>/p/bang-candy-apple-crisp-12-drinks/vz-2082</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_10 Ways Women Can Support Fertility Cross Promo Module', position : 'Cross Promo Module', name : '2003_10 Ways Women Can Support Fertility', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>https://whatsgood.vitaminshoppe.com/10-ways-women-can-support-their-fertility-naturally/</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Apparel Get in Gear Cross Promo Module', position : 'Cross Promo Module', name : '2003_Apparel Get in Gear', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Black Seed Oil Cross Promo Module', position : 'Cross Promo Module', name : '2003_Black Seed Oil', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Browse Videos Cross Promo Module', position : 'Cross Promo Module', name : '2003_Browse Videos', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Welcome to CBD Centeral  Cross Promo Module', position : 'Cross Promo Module', name : '2003_Welcome to CBD Centeral ', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_Curious About CBD Cross Promo Module', position : 'Cross Promo Module', name : '2003_Curious About CBD', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>10-Ways-Women-Can-Support-Their-Fertility-Naturally-BLOG-CPCM_06</t>
+  </si>
+  <si>
+    <t>Apparel_V2_A_CPCM_06</t>
+  </si>
+  <si>
+    <t>BangNewFlavor_CandyAppleCrisp_123019_CPCM_06</t>
+  </si>
+  <si>
+    <t>Black-Seed-Oil-101_CPCM_06</t>
+  </si>
+  <si>
+    <t>BROWSEOURVIDEOSCPCM_V1_A_CPCM-static_06</t>
+  </si>
+  <si>
+    <t>CBD-ASSET-UPDATE-62270_V2_A_CPCM_CPCM_0</t>
+  </si>
+  <si>
+    <t>CuriousAboutCBD_V1_A_CPCM_06</t>
+  </si>
+  <si>
+    <t>WHAT TO KNOW IF YOU'RE CURIOUS ABOUT TRYING CBD HEMP EXTRACT</t>
+  </si>
+  <si>
+    <t>From celebrity endorsers to licensed physicians, everybody's talking about CBD. But what exactly is it?</t>
+  </si>
+  <si>
+    <t>CHECK IT OUT &gt;</t>
+  </si>
+  <si>
+    <t>hemp</t>
+  </si>
+  <si>
+    <t>FIND THE CBD THAT'S RIGHT FOR YOU</t>
+  </si>
+  <si>
+    <t>LEARN MORE &gt;</t>
+  </si>
+  <si>
+    <t>cbd-central</t>
+  </si>
+  <si>
+    <t>The Vitamin Shoppe&lt;sup&gt;&amp;reg;&lt;/sup&gt; is your one-stop destination for CBD hemp extract from brands you can trust.</t>
+  </si>
+  <si>
+    <t>BROWSE OUR VIDEO GALLERY&amp;mdash;RECIPES, WORKOUTS &amp;amp; MORE!</t>
+  </si>
+  <si>
+    <t>Want some tips on your path to wellness? Watch these.</t>
+  </si>
+  <si>
+    <t>gallery</t>
+  </si>
+  <si>
+    <t>black-seed</t>
+  </si>
+  <si>
+    <t>apparel</t>
+  </si>
+  <si>
+    <t>fertility</t>
+  </si>
+  <si>
+    <t>bang</t>
+  </si>
+  <si>
+    <t>#E4E4E4</t>
+  </si>
+  <si>
+    <t>#D3DEC0</t>
+  </si>
+  <si>
+    <t>BLACK SEED OIL 101</t>
+  </si>
+  <si>
+    <t>SHOP BLACK SEED OILS&gt; &lt;Br&gt; &lt;br&gt; a &lt;a href=""&gt;SHOP OUR PICK: PLNT&lt;sup&gt;&amp;reg;&lt;/sup&gt; BRAND ORGANIC &gt;</t>
+  </si>
+  <si>
+    <t>Used for centuries in Ayurvedic medicine and Middle Eastern countries, black seed oil is a popular antioxidant for immune support and cellular health.</t>
+  </si>
+  <si>
+    <t>#886349</t>
+  </si>
+  <si>
+    <t>GET IN GEAR!</t>
+  </si>
+  <si>
+    <t>Now you can rep your squad with apparel from brands you love</t>
+  </si>
+  <si>
+    <t>FIND YOUR FIT&gt;</t>
+  </si>
+  <si>
+    <t>#FCFCFC</t>
+  </si>
+  <si>
+    <t>#B2B4CB</t>
+  </si>
+  <si>
+    <t>10 WAYS WOMEN CAN SUPPORT THEIR FERTILITY NATURALLY</t>
+  </si>
+  <si>
+    <t>Fertility issues at an all-tme high, so it's important that women find ways to support their reproductive health every day.</t>
+  </si>
+  <si>
+    <t>#F4CB93</t>
+  </si>
+  <si>
+    <t>New Bang Flavor Revealed: Candy Apple Crisp!</t>
+  </si>
+  <si>
+    <t>Fuel performance with BANG'S newest sugar-free energy drink feat. 300 mg caffeine, Super Creatine&lt;sup&gt;&amp;reg;&lt;/sup&gt; &amp;amp; EAAs!</t>
+  </si>
+  <si>
+    <t>SHOP NOW&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +525,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -361,7 +548,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -384,12 +571,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,6 +599,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -716,9 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B95EF76-0683-7442-8057-403F4623BCC9}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -923,6 +1124,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BC099C-CB2B-0E4A-8119-3E6C0EAF1566}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1197,4 +1399,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D0A18-1692-8545-B69B-D55DE77D3227}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{A2992379-05B9-5F47-938A-A43E9D04823C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>